<commit_message>
Completing Phase 3, and adding dates for Gannt Chart
</commit_message>
<xml_diff>
--- a/management/Gannt Chart.xlsx
+++ b/management/Gannt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="84">
   <si>
     <t>GANTT CHART TEMPLATE</t>
   </si>
@@ -266,6 +266,21 @@
   </si>
   <si>
     <t>Plan meeting for work distrubtion during phase 2 (Advanced)</t>
+  </si>
+  <si>
+    <t>Phase 3: Namespace Implementation - Statistical Functions</t>
+  </si>
+  <si>
+    <t>Plan meeting for work distrubtion during phase 3 (Advanced)</t>
+  </si>
+  <si>
+    <t>Write search-for-item by value namespace (Intermediate)</t>
+  </si>
+  <si>
+    <t>Write sorting algorithm namespace (Intermediate)</t>
+  </si>
+  <si>
+    <t>Write max/min/average price namespace (Intermediate)</t>
   </si>
 </sst>
 </file>
@@ -566,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -714,6 +729,10 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -726,23 +745,23 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,11 +1250,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="476094272"/>
-        <c:axId val="476096592"/>
+        <c:axId val="1313489952"/>
+        <c:axId val="1313492272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="476094272"/>
+        <c:axId val="1313489952"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1260,7 +1279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476096592"/>
+        <c:crossAx val="1313492272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1268,7 +1287,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="476096592"/>
+        <c:axId val="1313492272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1325,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1328,7 +1346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476094272"/>
+        <c:crossAx val="1313489952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1672,11 +1690,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="477151392"/>
-        <c:axId val="477154208"/>
+        <c:axId val="1313536848"/>
+        <c:axId val="1313539664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="477151392"/>
+        <c:axId val="1313536848"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1696,7 +1714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477154208"/>
+        <c:crossAx val="1313539664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1704,7 +1722,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="477154208"/>
+        <c:axId val="1313539664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1762,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1766,7 +1783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="477151392"/>
+        <c:crossAx val="1313536848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1798,7 +1815,7 @@
         <xdr:cNvPr id="2" name="Chart 2" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1835,7 +1852,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3CFC8EFD-7B6C-4413-BAAC-D7E8FADEB088}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CFC8EFD-7B6C-4413-BAAC-D7E8FADEB088}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1885,7 +1902,7 @@
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2420,80 +2437,80 @@
       <c r="AJ5" s="2"/>
     </row>
     <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="75"/>
+      <c r="B6" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="76" t="s">
+      <c r="K6" s="78"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="75" t="s">
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="74"/>
-      <c r="W6" s="74"/>
-      <c r="X6" s="74"/>
-      <c r="Y6" s="74"/>
-      <c r="Z6" s="76" t="s">
+      <c r="V6" s="76"/>
+      <c r="W6" s="76"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="AA6" s="74"/>
-      <c r="AB6" s="74"/>
-      <c r="AC6" s="74"/>
-      <c r="AD6" s="74"/>
-      <c r="AE6" s="75" t="s">
+      <c r="AA6" s="76"/>
+      <c r="AB6" s="76"/>
+      <c r="AC6" s="76"/>
+      <c r="AD6" s="76"/>
+      <c r="AE6" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="AF6" s="74"/>
-      <c r="AG6" s="74"/>
-      <c r="AH6" s="74"/>
-      <c r="AI6" s="74"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="76"/>
+      <c r="AH6" s="76"/>
+      <c r="AI6" s="76"/>
       <c r="AJ6" s="43"/>
     </row>
     <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
       <c r="M7" s="43"/>
@@ -3328,6 +3345,13 @@
     <row r="50" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="F6:F7"/>
@@ -3336,13 +3360,6 @@
     <mergeCell ref="U6:Y6"/>
     <mergeCell ref="K6:O6"/>
     <mergeCell ref="P6:T6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="J9:J13 J15:J18 J20:J24 J26:J29">
     <cfRule type="colorScale" priority="1">
@@ -3466,16 +3483,16 @@
       <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -3577,72 +3594,72 @@
       <c r="AH5" s="2"/>
     </row>
     <row r="6" spans="1:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="75"/>
+      <c r="B6" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="76" t="s">
+      <c r="I6" s="78"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="75" t="s">
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="74"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="74"/>
-      <c r="X6" s="76" t="s">
+      <c r="T6" s="76"/>
+      <c r="U6" s="76"/>
+      <c r="V6" s="76"/>
+      <c r="W6" s="76"/>
+      <c r="X6" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="74"/>
-      <c r="Z6" s="74"/>
-      <c r="AA6" s="74"/>
-      <c r="AB6" s="74"/>
-      <c r="AC6" s="75" t="s">
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="76"/>
+      <c r="AB6" s="76"/>
+      <c r="AC6" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="AD6" s="74"/>
-      <c r="AE6" s="74"/>
-      <c r="AF6" s="74"/>
-      <c r="AG6" s="74"/>
+      <c r="AD6" s="76"/>
+      <c r="AE6" s="76"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="76"/>
       <c r="AH6" s="43"/>
     </row>
     <row r="7" spans="1:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="43"/>
@@ -4319,11 +4336,6 @@
     <row r="50" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AC6:AG6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="N6:R6"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E6:E7"/>
@@ -4333,6 +4345,11 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="AC6:AG6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="N6:R6"/>
   </mergeCells>
   <conditionalFormatting sqref="H9:H13 H15:H18 H20:H24 H26:H29">
     <cfRule type="colorScale" priority="1">
@@ -4359,10 +4376,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO978"/>
+  <dimension ref="A1:BO977"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4514,15 +4531,15 @@
       <c r="BO2" s="2"/>
     </row>
     <row r="3" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -4723,118 +4740,118 @@
       <c r="BO5" s="2"/>
     </row>
     <row r="6" spans="1:67" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="75"/>
+      <c r="B6" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="84" t="s">
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="82" t="s">
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="84" t="s">
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
-      <c r="Z6" s="83"/>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="82" t="s">
+      <c r="X6" s="82"/>
+      <c r="Y6" s="82"/>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="82"/>
+      <c r="AB6" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="83"/>
-      <c r="AF6" s="83"/>
-      <c r="AG6" s="84" t="s">
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="82"/>
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="AH6" s="83"/>
-      <c r="AI6" s="83"/>
-      <c r="AJ6" s="83"/>
-      <c r="AK6" s="83"/>
-      <c r="AL6" s="82" t="s">
+      <c r="AH6" s="82"/>
+      <c r="AI6" s="82"/>
+      <c r="AJ6" s="82"/>
+      <c r="AK6" s="82"/>
+      <c r="AL6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="AM6" s="83"/>
-      <c r="AN6" s="83"/>
-      <c r="AO6" s="83"/>
-      <c r="AP6" s="83"/>
-      <c r="AQ6" s="84" t="s">
+      <c r="AM6" s="82"/>
+      <c r="AN6" s="82"/>
+      <c r="AO6" s="82"/>
+      <c r="AP6" s="82"/>
+      <c r="AQ6" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="AR6" s="83"/>
-      <c r="AS6" s="83"/>
-      <c r="AT6" s="83"/>
-      <c r="AU6" s="83"/>
-      <c r="AV6" s="82" t="s">
+      <c r="AR6" s="82"/>
+      <c r="AS6" s="82"/>
+      <c r="AT6" s="82"/>
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="AW6" s="83"/>
-      <c r="AX6" s="83"/>
-      <c r="AY6" s="83"/>
-      <c r="AZ6" s="83"/>
-      <c r="BA6" s="84" t="s">
+      <c r="AW6" s="82"/>
+      <c r="AX6" s="82"/>
+      <c r="AY6" s="82"/>
+      <c r="AZ6" s="82"/>
+      <c r="BA6" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="BB6" s="83"/>
-      <c r="BC6" s="83"/>
-      <c r="BD6" s="83"/>
-      <c r="BE6" s="83"/>
-      <c r="BF6" s="82" t="s">
+      <c r="BB6" s="82"/>
+      <c r="BC6" s="82"/>
+      <c r="BD6" s="82"/>
+      <c r="BE6" s="82"/>
+      <c r="BF6" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="BG6" s="83"/>
-      <c r="BH6" s="83"/>
-      <c r="BI6" s="83"/>
-      <c r="BJ6" s="83"/>
-      <c r="BK6" s="84" t="s">
+      <c r="BG6" s="82"/>
+      <c r="BH6" s="82"/>
+      <c r="BI6" s="82"/>
+      <c r="BJ6" s="82"/>
+      <c r="BK6" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="BL6" s="83"/>
-      <c r="BM6" s="83"/>
-      <c r="BN6" s="83"/>
-      <c r="BO6" s="83"/>
+      <c r="BL6" s="82"/>
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="82"/>
+      <c r="BO6" s="82"/>
     </row>
     <row r="7" spans="1:67" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="87"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
@@ -5021,11 +5038,11 @@
         <v>60</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
       <c r="J8" s="18"/>
@@ -5105,9 +5122,9 @@
         <v>57</v>
       </c>
       <c r="G9" s="22">
-        <v>1</v>
-      </c>
-      <c r="H9" s="23"/>
+        <v>0.9</v>
+      </c>
+      <c r="H9" s="31"/>
       <c r="I9" s="24"/>
       <c r="J9" s="25"/>
       <c r="K9" s="25"/>
@@ -5186,7 +5203,7 @@
         <v>73</v>
       </c>
       <c r="G10" s="29">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="24"/>
@@ -5253,8 +5270,12 @@
       <c r="B11" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="C11" s="37">
+        <v>47174</v>
+      </c>
+      <c r="D11" s="37">
+        <v>43521</v>
+      </c>
       <c r="E11" s="21"/>
       <c r="F11" s="19" t="s">
         <v>57</v>
@@ -5325,8 +5346,12 @@
       <c r="B12" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="C12" s="37">
+        <v>43522</v>
+      </c>
+      <c r="D12" s="37">
+        <v>43523</v>
+      </c>
       <c r="E12" s="21"/>
       <c r="F12" s="19" t="s">
         <v>58</v>
@@ -5398,10 +5423,10 @@
         <v>70</v>
       </c>
       <c r="C13" s="20">
-        <v>43517</v>
+        <v>43522</v>
       </c>
       <c r="D13" s="20">
-        <v>43518</v>
+        <v>43523</v>
       </c>
       <c r="E13" s="21">
         <f t="shared" si="0"/>
@@ -5411,17 +5436,17 @@
         <v>68</v>
       </c>
       <c r="G13" s="22">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
@@ -5478,8 +5503,12 @@
       <c r="B14" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="C14" s="37">
+        <v>43525</v>
+      </c>
+      <c r="D14" s="37">
+        <v>43529</v>
+      </c>
       <c r="E14" s="21"/>
       <c r="F14" s="19" t="s">
         <v>58</v>
@@ -5489,11 +5518,11 @@
       <c r="I14" s="24"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
@@ -5550,8 +5579,12 @@
       <c r="B15" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="C15" s="37">
+        <v>43525</v>
+      </c>
+      <c r="D15" s="37">
+        <v>43529</v>
+      </c>
       <c r="E15" s="21"/>
       <c r="F15" s="19" t="s">
         <v>57</v>
@@ -5561,11 +5594,11 @@
       <c r="I15" s="24"/>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
       <c r="Q15" s="26"/>
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
@@ -5622,8 +5655,12 @@
       <c r="B16" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="C16" s="37">
+        <v>43525</v>
+      </c>
+      <c r="D16" s="37">
+        <v>43529</v>
+      </c>
       <c r="E16" s="21"/>
       <c r="F16" s="19" t="s">
         <v>68</v>
@@ -5633,11 +5670,11 @@
       <c r="I16" s="24"/>
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
@@ -5694,17 +5731,21 @@
       <c r="B17" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="20">
+        <v>43525</v>
+      </c>
+      <c r="D17" s="20">
+        <v>43529</v>
+      </c>
       <c r="E17" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>57</v>
       </c>
       <c r="G17" s="32">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="24"/>
@@ -5712,11 +5753,11 @@
       <c r="K17" s="25"/>
       <c r="L17" s="25"/>
       <c r="M17" s="26"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
@@ -5771,8 +5812,12 @@
       <c r="B18" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
+      <c r="C18" s="37">
+        <v>43525</v>
+      </c>
+      <c r="D18" s="37">
+        <v>43529</v>
+      </c>
       <c r="E18" s="21"/>
       <c r="F18" s="19" t="s">
         <v>58</v>
@@ -5784,11 +5829,11 @@
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
       <c r="M18" s="26"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="25"/>
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="25"/>
@@ -5843,17 +5888,21 @@
       <c r="B19" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="20">
+        <v>43529</v>
+      </c>
+      <c r="D19" s="20">
+        <v>43531</v>
+      </c>
       <c r="E19" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>57</v>
       </c>
       <c r="G19" s="33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="23"/>
       <c r="I19" s="24"/>
@@ -5863,11 +5912,11 @@
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
       <c r="W19" s="26"/>
@@ -5921,11 +5970,11 @@
         <v>76</v>
       </c>
       <c r="B20" s="70"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
       <c r="H20" s="34"/>
       <c r="I20" s="35"/>
       <c r="J20" s="36"/>
@@ -5987,13 +6036,17 @@
       <c r="BN20" s="34"/>
       <c r="BO20" s="34"/>
     </row>
-    <row r="21" spans="1:67" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:67" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="47"/>
       <c r="B21" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="C21" s="37">
+        <v>43531</v>
+      </c>
+      <c r="D21" s="37">
+        <v>43532</v>
+      </c>
       <c r="E21" s="21"/>
       <c r="F21" s="19" t="s">
         <v>58</v>
@@ -6066,20 +6119,20 @@
         <v>74</v>
       </c>
       <c r="C22" s="37">
-        <v>43517</v>
+        <v>43534</v>
       </c>
       <c r="D22" s="37">
-        <v>43520</v>
+        <v>43539</v>
       </c>
       <c r="E22" s="21">
         <f>NETWORKDAYS(C22,D22)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G22" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
@@ -6148,18 +6201,20 @@
         <v>75</v>
       </c>
       <c r="C23" s="37">
-        <v>43521</v>
+        <v>43534</v>
       </c>
       <c r="D23" s="37">
-        <v>43524</v>
+        <v>43539</v>
       </c>
       <c r="E23" s="21">
         <f t="shared" ref="E23" si="1">NETWORKDAYS(C23,D23)</f>
-        <v>4</v>
-      </c>
-      <c r="F23" s="19"/>
+        <v>5</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>68</v>
+      </c>
       <c r="G23" s="29">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="24"/>
@@ -6227,8 +6282,12 @@
       <c r="B24" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="C24" s="37">
+        <v>43534</v>
+      </c>
+      <c r="D24" s="37">
+        <v>43539</v>
+      </c>
       <c r="E24" s="21"/>
       <c r="F24" s="19" t="s">
         <v>57</v>
@@ -6295,20 +6354,394 @@
       <c r="BN24" s="26"/>
       <c r="BO24" s="28"/>
     </row>
-    <row r="25" spans="1:67" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="47"/>
-    </row>
-    <row r="26" spans="1:67" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:67" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="74"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="34"/>
+      <c r="X25" s="34"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="34"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="34"/>
+      <c r="AE25" s="34"/>
+      <c r="AF25" s="34"/>
+      <c r="AG25" s="34"/>
+      <c r="AH25" s="34"/>
+      <c r="AI25" s="34"/>
+      <c r="AJ25" s="34"/>
+      <c r="AK25" s="34"/>
+      <c r="AL25" s="34"/>
+      <c r="AM25" s="34"/>
+      <c r="AN25" s="34"/>
+      <c r="AO25" s="34"/>
+      <c r="AP25" s="34"/>
+      <c r="AQ25" s="34"/>
+      <c r="AR25" s="34"/>
+      <c r="AS25" s="34"/>
+      <c r="AT25" s="34"/>
+      <c r="AU25" s="34"/>
+      <c r="AV25" s="34"/>
+      <c r="AW25" s="34"/>
+      <c r="AX25" s="34"/>
+      <c r="AY25" s="34"/>
+      <c r="AZ25" s="34"/>
+      <c r="BA25" s="34"/>
+      <c r="BB25" s="34"/>
+      <c r="BC25" s="34"/>
+      <c r="BD25" s="34"/>
+      <c r="BE25" s="34"/>
+      <c r="BF25" s="34"/>
+      <c r="BG25" s="34"/>
+      <c r="BH25" s="34"/>
+      <c r="BI25" s="34"/>
+      <c r="BJ25" s="34"/>
+      <c r="BK25" s="34"/>
+      <c r="BL25" s="34"/>
+      <c r="BM25" s="34"/>
+      <c r="BN25" s="34"/>
+      <c r="BO25" s="34"/>
+    </row>
+    <row r="26" spans="1:67" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="47"/>
-    </row>
-    <row r="27" spans="1:67" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="47"/>
-    </row>
-    <row r="28" spans="1:67" ht="13" x14ac:dyDescent="0.15">
+      <c r="B26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="37">
+        <v>43539</v>
+      </c>
+      <c r="D26" s="37">
+        <v>43540</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="27"/>
+      <c r="AC26" s="27"/>
+      <c r="AD26" s="27"/>
+      <c r="AE26" s="27"/>
+      <c r="AF26" s="27"/>
+      <c r="AG26" s="26"/>
+      <c r="AH26" s="26"/>
+      <c r="AI26" s="26"/>
+      <c r="AJ26" s="26"/>
+      <c r="AK26" s="26"/>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="27"/>
+      <c r="AP26" s="27"/>
+      <c r="AQ26" s="26"/>
+      <c r="AR26" s="26"/>
+      <c r="AS26" s="26"/>
+      <c r="AT26" s="26"/>
+      <c r="AU26" s="26"/>
+      <c r="AV26" s="25"/>
+      <c r="AW26" s="25"/>
+      <c r="AX26" s="25"/>
+      <c r="AY26" s="25"/>
+      <c r="AZ26" s="25"/>
+      <c r="BA26" s="26"/>
+      <c r="BB26" s="26"/>
+      <c r="BC26" s="26"/>
+      <c r="BD26" s="26"/>
+      <c r="BE26" s="26"/>
+      <c r="BF26" s="27"/>
+      <c r="BG26" s="27"/>
+      <c r="BH26" s="27"/>
+      <c r="BI26" s="27"/>
+      <c r="BJ26" s="27"/>
+      <c r="BK26" s="26"/>
+      <c r="BL26" s="26"/>
+      <c r="BM26" s="26"/>
+      <c r="BN26" s="26"/>
+      <c r="BO26" s="28"/>
+    </row>
+    <row r="27" spans="1:67" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="45"/>
+      <c r="B27" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="37">
+        <v>43541</v>
+      </c>
+      <c r="D27" s="37">
+        <v>43544</v>
+      </c>
+      <c r="E27" s="21">
+        <f>NETWORKDAYS(C27,D27)</f>
+        <v>3</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="22">
+        <v>0</v>
+      </c>
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="26"/>
+      <c r="Z27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="27"/>
+      <c r="AC27" s="27"/>
+      <c r="AD27" s="27"/>
+      <c r="AE27" s="27"/>
+      <c r="AF27" s="27"/>
+      <c r="AG27" s="26"/>
+      <c r="AH27" s="26"/>
+      <c r="AI27" s="26"/>
+      <c r="AJ27" s="26"/>
+      <c r="AK27" s="26"/>
+      <c r="AL27" s="27"/>
+      <c r="AM27" s="27"/>
+      <c r="AN27" s="27"/>
+      <c r="AO27" s="27"/>
+      <c r="AP27" s="27"/>
+      <c r="AQ27" s="26"/>
+      <c r="AR27" s="26"/>
+      <c r="AS27" s="26"/>
+      <c r="AT27" s="26"/>
+      <c r="AU27" s="26"/>
+      <c r="AV27" s="25"/>
+      <c r="AW27" s="25"/>
+      <c r="AX27" s="25"/>
+      <c r="AY27" s="25"/>
+      <c r="AZ27" s="25"/>
+      <c r="BA27" s="26"/>
+      <c r="BB27" s="26"/>
+      <c r="BC27" s="26"/>
+      <c r="BD27" s="26"/>
+      <c r="BE27" s="26"/>
+      <c r="BF27" s="27"/>
+      <c r="BG27" s="27"/>
+      <c r="BH27" s="27"/>
+      <c r="BI27" s="27"/>
+      <c r="BJ27" s="27"/>
+      <c r="BK27" s="26"/>
+      <c r="BL27" s="26"/>
+      <c r="BM27" s="26"/>
+      <c r="BN27" s="26"/>
+      <c r="BO27" s="28"/>
+    </row>
+    <row r="28" spans="1:67" s="73" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="47"/>
-    </row>
-    <row r="29" spans="1:67" ht="13" x14ac:dyDescent="0.15">
+      <c r="B28" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="37">
+        <v>43541</v>
+      </c>
+      <c r="D28" s="37">
+        <v>43544</v>
+      </c>
+      <c r="E28" s="21">
+        <f t="shared" ref="E28" si="2">NETWORKDAYS(C28,D28)</f>
+        <v>3</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="29">
+        <v>0</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="25"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="27"/>
+      <c r="AC28" s="27"/>
+      <c r="AD28" s="27"/>
+      <c r="AE28" s="27"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="26"/>
+      <c r="AH28" s="26"/>
+      <c r="AI28" s="26"/>
+      <c r="AJ28" s="26"/>
+      <c r="AK28" s="26"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="27"/>
+      <c r="AO28" s="27"/>
+      <c r="AP28" s="27"/>
+      <c r="AQ28" s="26"/>
+      <c r="AR28" s="26"/>
+      <c r="AS28" s="26"/>
+      <c r="AT28" s="26"/>
+      <c r="AU28" s="26"/>
+      <c r="AV28" s="25"/>
+      <c r="AW28" s="25"/>
+      <c r="AX28" s="25"/>
+      <c r="AY28" s="25"/>
+      <c r="AZ28" s="25"/>
+      <c r="BA28" s="26"/>
+      <c r="BB28" s="26"/>
+      <c r="BC28" s="26"/>
+      <c r="BD28" s="26"/>
+      <c r="BE28" s="26"/>
+      <c r="BF28" s="27"/>
+      <c r="BG28" s="27"/>
+      <c r="BH28" s="27"/>
+      <c r="BI28" s="27"/>
+      <c r="BJ28" s="27"/>
+      <c r="BK28" s="26"/>
+      <c r="BL28" s="26"/>
+      <c r="BM28" s="26"/>
+      <c r="BN28" s="26"/>
+      <c r="BO28" s="28"/>
+    </row>
+    <row r="29" spans="1:67" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="47"/>
+      <c r="B29" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="37">
+        <v>43541</v>
+      </c>
+      <c r="D29" s="37">
+        <v>43544</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="29"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="27"/>
+      <c r="AC29" s="27"/>
+      <c r="AD29" s="27"/>
+      <c r="AE29" s="27"/>
+      <c r="AF29" s="27"/>
+      <c r="AG29" s="26"/>
+      <c r="AH29" s="26"/>
+      <c r="AI29" s="26"/>
+      <c r="AJ29" s="26"/>
+      <c r="AK29" s="26"/>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="27"/>
+      <c r="AO29" s="27"/>
+      <c r="AP29" s="27"/>
+      <c r="AQ29" s="26"/>
+      <c r="AR29" s="26"/>
+      <c r="AS29" s="26"/>
+      <c r="AT29" s="26"/>
+      <c r="AU29" s="26"/>
+      <c r="AV29" s="25"/>
+      <c r="AW29" s="25"/>
+      <c r="AX29" s="25"/>
+      <c r="AY29" s="25"/>
+      <c r="AZ29" s="25"/>
+      <c r="BA29" s="26"/>
+      <c r="BB29" s="26"/>
+      <c r="BC29" s="26"/>
+      <c r="BD29" s="26"/>
+      <c r="BE29" s="26"/>
+      <c r="BF29" s="27"/>
+      <c r="BG29" s="27"/>
+      <c r="BH29" s="27"/>
+      <c r="BI29" s="27"/>
+      <c r="BJ29" s="27"/>
+      <c r="BK29" s="26"/>
+      <c r="BL29" s="26"/>
+      <c r="BM29" s="26"/>
+      <c r="BN29" s="26"/>
+      <c r="BO29" s="28"/>
     </row>
     <row r="30" spans="1:67" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="47"/>
@@ -9078,69 +9511,69 @@
     </row>
     <row r="952" spans="1:67" ht="13" x14ac:dyDescent="0.15">
       <c r="A952" s="47"/>
+      <c r="H952" s="4"/>
+      <c r="I952" s="4"/>
+      <c r="J952" s="4"/>
+      <c r="K952" s="4"/>
+      <c r="L952" s="4"/>
+      <c r="M952" s="4"/>
+      <c r="N952" s="4"/>
+      <c r="O952" s="4"/>
+      <c r="P952" s="4"/>
+      <c r="Q952" s="4"/>
+      <c r="R952" s="4"/>
+      <c r="S952" s="4"/>
+      <c r="T952" s="4"/>
+      <c r="U952" s="4"/>
+      <c r="V952" s="4"/>
+      <c r="W952" s="4"/>
+      <c r="X952" s="4"/>
+      <c r="Y952" s="4"/>
+      <c r="Z952" s="4"/>
+      <c r="AA952" s="4"/>
+      <c r="AB952" s="4"/>
+      <c r="AC952" s="4"/>
+      <c r="AD952" s="4"/>
+      <c r="AE952" s="4"/>
+      <c r="AF952" s="4"/>
+      <c r="AG952" s="4"/>
+      <c r="AH952" s="4"/>
+      <c r="AI952" s="4"/>
+      <c r="AJ952" s="4"/>
+      <c r="AK952" s="4"/>
+      <c r="AL952" s="4"/>
+      <c r="AM952" s="4"/>
+      <c r="AN952" s="4"/>
+      <c r="AO952" s="4"/>
+      <c r="AP952" s="4"/>
+      <c r="AQ952" s="4"/>
+      <c r="AR952" s="4"/>
+      <c r="AS952" s="4"/>
+      <c r="AT952" s="4"/>
+      <c r="AU952" s="4"/>
+      <c r="AV952" s="4"/>
+      <c r="AW952" s="4"/>
+      <c r="AX952" s="4"/>
+      <c r="AY952" s="4"/>
+      <c r="AZ952" s="4"/>
+      <c r="BA952" s="4"/>
+      <c r="BB952" s="4"/>
+      <c r="BC952" s="4"/>
+      <c r="BD952" s="4"/>
+      <c r="BE952" s="4"/>
+      <c r="BF952" s="4"/>
+      <c r="BG952" s="4"/>
+      <c r="BH952" s="4"/>
+      <c r="BI952" s="4"/>
+      <c r="BJ952" s="4"/>
+      <c r="BK952" s="4"/>
+      <c r="BL952" s="4"/>
+      <c r="BM952" s="4"/>
+      <c r="BN952" s="4"/>
+      <c r="BO952" s="4"/>
     </row>
     <row r="953" spans="1:67" ht="13" x14ac:dyDescent="0.15">
       <c r="A953" s="47"/>
-      <c r="H953" s="4"/>
-      <c r="I953" s="4"/>
-      <c r="J953" s="4"/>
-      <c r="K953" s="4"/>
-      <c r="L953" s="4"/>
-      <c r="M953" s="4"/>
-      <c r="N953" s="4"/>
-      <c r="O953" s="4"/>
-      <c r="P953" s="4"/>
-      <c r="Q953" s="4"/>
-      <c r="R953" s="4"/>
-      <c r="S953" s="4"/>
-      <c r="T953" s="4"/>
-      <c r="U953" s="4"/>
-      <c r="V953" s="4"/>
-      <c r="W953" s="4"/>
-      <c r="X953" s="4"/>
-      <c r="Y953" s="4"/>
-      <c r="Z953" s="4"/>
-      <c r="AA953" s="4"/>
-      <c r="AB953" s="4"/>
-      <c r="AC953" s="4"/>
-      <c r="AD953" s="4"/>
-      <c r="AE953" s="4"/>
-      <c r="AF953" s="4"/>
-      <c r="AG953" s="4"/>
-      <c r="AH953" s="4"/>
-      <c r="AI953" s="4"/>
-      <c r="AJ953" s="4"/>
-      <c r="AK953" s="4"/>
-      <c r="AL953" s="4"/>
-      <c r="AM953" s="4"/>
-      <c r="AN953" s="4"/>
-      <c r="AO953" s="4"/>
-      <c r="AP953" s="4"/>
-      <c r="AQ953" s="4"/>
-      <c r="AR953" s="4"/>
-      <c r="AS953" s="4"/>
-      <c r="AT953" s="4"/>
-      <c r="AU953" s="4"/>
-      <c r="AV953" s="4"/>
-      <c r="AW953" s="4"/>
-      <c r="AX953" s="4"/>
-      <c r="AY953" s="4"/>
-      <c r="AZ953" s="4"/>
-      <c r="BA953" s="4"/>
-      <c r="BB953" s="4"/>
-      <c r="BC953" s="4"/>
-      <c r="BD953" s="4"/>
-      <c r="BE953" s="4"/>
-      <c r="BF953" s="4"/>
-      <c r="BG953" s="4"/>
-      <c r="BH953" s="4"/>
-      <c r="BI953" s="4"/>
-      <c r="BJ953" s="4"/>
-      <c r="BK953" s="4"/>
-      <c r="BL953" s="4"/>
-      <c r="BM953" s="4"/>
-      <c r="BN953" s="4"/>
-      <c r="BO953" s="4"/>
     </row>
     <row r="954" spans="1:67" ht="13" x14ac:dyDescent="0.15">
       <c r="A954" s="47"/>
@@ -9206,21 +9639,25 @@
       <c r="A974" s="47"/>
     </row>
     <row r="975" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A975" s="47"/>
-    </row>
-    <row r="976" spans="1:7" ht="13" x14ac:dyDescent="0.15">
-      <c r="A976" s="67"/>
-      <c r="C976" s="4"/>
-      <c r="D976" s="4"/>
-      <c r="E976" s="4"/>
-      <c r="F976" s="4"/>
-      <c r="G976" s="4"/>
-    </row>
-    <row r="978" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B978" s="4"/>
+      <c r="A975" s="67"/>
+      <c r="C975" s="4"/>
+      <c r="D975" s="4"/>
+      <c r="E975" s="4"/>
+      <c r="F975" s="4"/>
+      <c r="G975" s="4"/>
+    </row>
+    <row r="977" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B977" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="BF6:BJ6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="W6:AA6"/>
     <mergeCell ref="BK6:BO6"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="A3:G3"/>
@@ -9237,15 +9674,9 @@
     <mergeCell ref="AG6:AK6"/>
     <mergeCell ref="AB6:AF6"/>
     <mergeCell ref="R6:V6"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="BF6:BJ6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="W6:AA6"/>
-    <mergeCell ref="C20:G20"/>
   </mergeCells>
   <conditionalFormatting sqref="G9:G19">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -9255,6 +9686,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF5CBCD6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:G24">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF5CBCD6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -9264,8 +9715,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22:G24">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="G27:G29">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>

</xml_diff>

<commit_message>
Added templates/campus directory and index.html
</commit_message>
<xml_diff>
--- a/management/Gannt Chart.xlsx
+++ b/management/Gannt Chart.xlsx
@@ -4379,7 +4379,7 @@
   <dimension ref="A1:BO977"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5280,7 +5280,9 @@
       <c r="F11" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="29"/>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
       <c r="H11" s="23"/>
       <c r="I11" s="24"/>
       <c r="J11" s="25"/>
@@ -5356,7 +5358,9 @@
       <c r="F12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
       <c r="J12" s="25"/>
@@ -5513,7 +5517,9 @@
       <c r="F14" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="22">
+        <v>0</v>
+      </c>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
       <c r="J14" s="25"/>
@@ -5589,7 +5595,9 @@
       <c r="F15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="22">
+        <v>0</v>
+      </c>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
       <c r="J15" s="25"/>
@@ -5665,7 +5673,9 @@
       <c r="F16" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="22">
+        <v>0</v>
+      </c>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
       <c r="J16" s="25"/>
@@ -5822,7 +5832,9 @@
       <c r="F18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="32">
+        <v>0</v>
+      </c>
       <c r="H18" s="23"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25"/>
@@ -6051,7 +6063,9 @@
       <c r="F21" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="29"/>
+      <c r="G21" s="29">
+        <v>0</v>
+      </c>
       <c r="H21" s="23"/>
       <c r="I21" s="24"/>
       <c r="J21" s="25"/>
@@ -6292,7 +6306,9 @@
       <c r="F24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="29"/>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
       <c r="J24" s="25"/>
@@ -6440,7 +6456,9 @@
       <c r="F26" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G26" s="29"/>
+      <c r="G26" s="29">
+        <v>0</v>
+      </c>
       <c r="H26" s="23"/>
       <c r="I26" s="24"/>
       <c r="J26" s="25"/>
@@ -6681,7 +6699,9 @@
       <c r="F29" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="29"/>
+      <c r="G29" s="29">
+        <v>0</v>
+      </c>
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
       <c r="J29" s="25"/>

</xml_diff>